<commit_message>
Update of all scripts and data
</commit_message>
<xml_diff>
--- a/OnBoard/data/fogli_cala/StationTablet_12.xlsx
+++ b/OnBoard/data/fogli_cala/StationTablet_12.xlsx
@@ -1,44 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\OneDrive - CNR\CNR\SoleMon\solemon2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc.MSI\Desktop\Github2024\SoleMon_project\OnBoard\data\fogli_cala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{8CE68332-AB83-474B-94DD-F272FF9602B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209AB71B-14B6-4E60-B299-9C5916B44A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="14400" windowHeight="9080" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Station" sheetId="1" r:id="rId1"/>
     <sheet name="NotesCala" sheetId="2" r:id="rId2"/>
     <sheet name="Samples onboard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>WindDirection</t>
   </si>
@@ -115,12 +104,6 @@
     <t>Notes shells</t>
   </si>
   <si>
-    <t>Lenght</t>
-  </si>
-  <si>
-    <t>Total weight</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -194,6 +177,15 @@
   </si>
   <si>
     <t>cavo 90 passi giri motore 920, parte sogliole rapi a misurate a bordo</t>
+  </si>
+  <si>
+    <t>Lenght_mm</t>
+  </si>
+  <si>
+    <t>Weight_g</t>
+  </si>
+  <si>
+    <t>Total weight_g</t>
   </si>
 </sst>
 </file>
@@ -314,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -349,10 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -635,34 +624,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7421875" style="13"/>
-    <col min="2" max="2" width="13.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.87109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.68359375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.28125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.0859375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.953125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="7.3984375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.2578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="13"/>
+    <col min="2" max="2" width="13.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="7.36328125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.6328125" style="6" customWidth="1"/>
     <col min="12" max="12" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.8359375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" style="6" customWidth="1"/>
-    <col min="15" max="15" width="11.703125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" style="6" customWidth="1"/>
-    <col min="17" max="17" width="13.44921875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="8.47265625" style="6" customWidth="1"/>
-    <col min="19" max="21" width="8.609375" style="6"/>
-    <col min="22" max="22" width="13.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="13.81640625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="8.453125" style="6" customWidth="1"/>
+    <col min="19" max="21" width="8.6328125" style="6"/>
+    <col min="22" max="22" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
@@ -688,13 +677,13 @@
         <v>19</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>0</v>
@@ -726,11 +715,11 @@
       <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="13">
         <v>12</v>
       </c>
@@ -765,19 +754,19 @@
         <v>205</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="P2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="10">
         <v>0.3611111111111111</v>
@@ -794,16 +783,16 @@
       <c r="U2" s="6">
         <v>32.204000000000001</v>
       </c>
-      <c r="V2" s="23">
+      <c r="V2">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D11" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="22:27" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
@@ -811,7 +800,7 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
     </row>
-    <row r="22" spans="22:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
@@ -832,19 +821,19 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7421875" style="9"/>
-    <col min="2" max="3" width="11.296875" style="6" customWidth="1"/>
-    <col min="4" max="5" width="11.703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.23828125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="13.85546875" style="6" customWidth="1"/>
-    <col min="9" max="10" width="10.4921875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="11.8359375" style="17" customWidth="1"/>
-    <col min="12" max="12" width="11.02734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="9"/>
+    <col min="2" max="3" width="11.26953125" style="6" customWidth="1"/>
+    <col min="4" max="5" width="11.7265625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="13.81640625" style="6" customWidth="1"/>
+    <col min="9" max="10" width="10.453125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="11" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -852,13 +841,13 @@
         <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -867,7 +856,7 @@
         <v>22</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>8</v>
@@ -882,7 +871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <f>Station!A2</f>
         <v>12</v>
@@ -900,496 +889,496 @@
         <v>110</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" s="6">
         <v>3.1</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <f>Station!A3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <f>Station!A4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <f>Station!A5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <f>Station!A6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <f>Station!A7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <f>Station!A8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <f>Station!A9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f>Station!A10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <f>Station!A11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <f>Station!A12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <f>Station!A13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <f>Station!A14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <f>Station!A15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <f>Station!A16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <f>Station!A17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <f>Station!A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <f>Station!A19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <f>Station!A20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <f>Station!A21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <f>Station!A22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <f>Station!A23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <f>Station!A24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <f>Station!A25</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <f>Station!A26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <f>Station!A27</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <f>Station!A28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <f>Station!A29</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <f>Station!A30</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <f>Station!A31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <f>Station!A32</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <f>Station!A33</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="9">
         <f>Station!A34</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="9">
         <f>Station!A35</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
         <f>Station!A36</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="9">
         <f>Station!A37</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="9">
         <f>Station!A38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <f>Station!A39</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
         <f>Station!A40</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
         <f>Station!A41</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
         <f>Station!A42</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
         <f>Station!A43</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
         <f>Station!A44</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="9">
         <f>Station!A45</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
         <f>Station!A46</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
         <f>Station!A47</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
         <f>Station!A48</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
         <f>Station!A49</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
         <f>Station!A50</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
         <f>Station!A51</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="9">
         <f>Station!A52</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="9">
         <f>Station!A53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
         <f>Station!A54</f>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
         <f>Station!A55</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="9">
         <f>Station!A56</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
         <f>Station!A57</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
         <f>Station!A58</f>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="9">
         <f>Station!A59</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
         <f>Station!A60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="9">
         <f>Station!A61</f>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="9">
         <f>Station!A62</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="9">
         <f>Station!A63</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="9">
         <f>Station!A64</f>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="9">
         <f>Station!A65</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="9">
         <f>Station!A66</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="9">
         <f>Station!A67</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="9">
         <f>Station!A68</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="9">
         <f>Station!A69</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="9">
         <f>Station!A70</f>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="9">
         <f>Station!A71</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="9">
         <f>Station!A72</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="9">
         <f>Station!A73</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="9">
         <f>Station!A74</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="9">
         <f>Station!A75</f>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="9">
         <f>Station!A76</f>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="9">
         <f>Station!A77</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="9">
         <f>Station!A78</f>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="9">
         <f>Station!A79</f>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="9">
         <f>Station!A80</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="9">
         <f>Station!A81</f>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="9">
         <f>Station!A82</f>
         <v>0</v>
@@ -1402,718 +1391,723 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639A9272-1023-F34A-8D2B-32933A221EB7}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="5" width="8.609375" style="18"/>
-    <col min="6" max="6" width="10.89453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.6328125" style="18"/>
+    <col min="4" max="4" width="10.90625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.6328125" style="18"/>
+    <col min="7" max="7" width="7.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="18">
         <v>166</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="18">
-        <v>1</v>
+      <c r="D2" s="18">
+        <v>40</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F2" s="18">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C3" s="18">
         <v>156</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="18">
-        <v>1</v>
+      <c r="D3" s="18">
+        <v>35</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F3" s="18">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C4" s="18">
         <v>240</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="D4" s="18">
+        <v>132</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="18">
         <v>2</v>
       </c>
-      <c r="F4" s="18">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C5" s="18">
         <v>183</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="18">
-        <v>1</v>
+      <c r="D5" s="18">
+        <v>56</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F5" s="18">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C6" s="18">
         <v>244</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="D6" s="18">
+        <v>132</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="18">
         <v>2</v>
       </c>
-      <c r="F6" s="18">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C7" s="18">
         <v>247</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="D7" s="18">
+        <v>156</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="18">
         <v>2</v>
       </c>
-      <c r="F7" s="18">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C8" s="18">
         <v>181</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="18">
-        <v>1</v>
+      <c r="D8" s="18">
+        <v>49</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F8" s="18">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C9" s="18">
         <v>242</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="D9" s="18">
+        <v>130</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="18">
         <v>2</v>
       </c>
-      <c r="F9" s="18">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C10" s="18">
         <v>174</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="18">
-        <v>1</v>
+      <c r="D10" s="18">
+        <v>52</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F10" s="18">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C11" s="18">
         <v>173</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="18">
-        <v>1</v>
+      <c r="D11" s="18">
+        <v>43</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F11" s="18">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C12" s="18">
         <v>172</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="18">
-        <v>1</v>
+      <c r="D12" s="18">
+        <v>46</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F12" s="18">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C13" s="18">
         <v>185</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="18">
-        <v>1</v>
+      <c r="D13" s="18">
+        <v>59</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F13" s="18">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C14" s="18">
         <v>241</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="18">
+      <c r="D14" s="18">
+        <v>137</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="18">
         <v>2</v>
       </c>
-      <c r="F14" s="18">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" s="18">
         <v>159</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="18">
-        <v>1</v>
+      <c r="D15" s="18">
+        <v>36</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F15" s="18">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C16" s="18">
         <v>153</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="18">
-        <v>1</v>
+      <c r="D16" s="18">
+        <v>37</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F16" s="18">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C17" s="18">
         <v>160</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="18">
-        <v>1</v>
+      <c r="D17" s="18">
+        <v>38</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F17" s="18">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C18" s="18">
         <v>181</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="18">
-        <v>1</v>
+      <c r="D18" s="18">
+        <v>51</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F18" s="18">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C19" s="18">
         <v>230</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="18">
+      <c r="D19" s="18">
+        <v>128</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="18">
         <v>2</v>
       </c>
-      <c r="F19" s="18">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C20" s="18">
         <v>241</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="18">
+      <c r="D20" s="18">
+        <v>134</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="18">
         <v>2</v>
       </c>
-      <c r="F20" s="18">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C21" s="18">
         <v>168</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="18">
-        <v>1</v>
+      <c r="D21" s="18">
+        <v>47</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F21" s="18">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C22" s="18">
         <v>240</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="18">
+      <c r="D22" s="18">
+        <v>118</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="18">
         <v>2</v>
       </c>
-      <c r="F22" s="18">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C23" s="18">
         <v>232</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="D23" s="18">
+        <v>114</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="18">
         <v>2</v>
       </c>
-      <c r="F23" s="18">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C24" s="18">
         <v>230</v>
       </c>
-      <c r="D24" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="18">
+      <c r="D24" s="18">
+        <v>125</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="18">
         <v>3</v>
       </c>
-      <c r="F24" s="18">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C25" s="18">
         <v>246</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="18">
+      <c r="D25" s="18">
+        <v>145</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="18">
         <v>3</v>
       </c>
-      <c r="F25" s="18">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C26" s="18">
         <v>185</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="18">
-        <v>1</v>
+      <c r="D26" s="18">
+        <v>63</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F26" s="18">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C27" s="18">
         <v>166</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="18">
-        <v>1</v>
+      <c r="D27" s="18">
+        <v>43</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F27" s="18">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C28" s="18">
         <v>170</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="18">
-        <v>1</v>
+      <c r="D28" s="18">
+        <v>45</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F28" s="18">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C29" s="18">
         <v>178</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="18">
-        <v>1</v>
+      <c r="D29" s="18">
+        <v>51</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F29" s="18">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C30" s="18">
         <v>167</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="18">
-        <v>1</v>
+      <c r="D30" s="18">
+        <v>48</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F30" s="18">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C31" s="18">
         <v>170</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="18">
-        <v>1</v>
+      <c r="D31" s="18">
+        <v>49</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F31" s="18">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C32" s="18">
         <v>193</v>
       </c>
-      <c r="D32" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="18">
+      <c r="D32" s="18">
+        <v>68</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="18">
         <v>2</v>
       </c>
-      <c r="F32" s="18">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C33" s="18">
         <v>192</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="18">
-        <v>1</v>
+      <c r="D33" s="18">
+        <v>69</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F33" s="18">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C34" s="18">
         <v>262</v>
       </c>
-      <c r="D34" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="18">
+      <c r="D34" s="18">
+        <v>167</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="18">
         <v>2</v>
       </c>
-      <c r="F34" s="18">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C35" s="18">
         <v>231</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="18">
+      <c r="D35" s="18">
+        <v>105</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="18">
         <v>2</v>
       </c>
-      <c r="F35" s="18">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C36" s="18">
         <v>184</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="18">
-        <v>1</v>
+      <c r="D36" s="18">
+        <v>52</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F36" s="18">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C37" s="18">
         <v>165</v>
       </c>
-      <c r="D37" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="18">
-        <v>1</v>
+      <c r="D37" s="18">
+        <v>45</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F37" s="18">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C38" s="18">
         <v>168</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="18">
-        <v>1</v>
+      <c r="D38" s="18">
+        <v>43</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F38" s="18">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C39" s="18">
         <v>236</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="18">
+      <c r="D39" s="18">
+        <v>108</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="18">
         <v>2</v>
       </c>
-      <c r="F39" s="18">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C40" s="18">
         <v>185</v>
       </c>
-      <c r="D40" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="18">
-        <v>1</v>
+      <c r="D40" s="18">
+        <v>55</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F40" s="18">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C41" s="18">
         <v>248</v>
       </c>
-      <c r="D41" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="18">
+      <c r="D41" s="18">
+        <v>146</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="18">
         <v>2</v>
       </c>
-      <c r="F41" s="18">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C42" s="18">
         <v>240</v>
       </c>
-      <c r="D42" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E42" s="18">
+      <c r="D42" s="18">
+        <v>117</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="18">
         <v>2</v>
       </c>
-      <c r="F42" s="18">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C43" s="18">
         <v>180</v>
       </c>
-      <c r="D43" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="18">
-        <v>1</v>
+      <c r="D43" s="18">
+        <v>44</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F43" s="18">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C44" s="18">
         <v>164</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="18">
-        <v>1</v>
+      <c r="D44" s="18">
+        <v>46</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F44" s="18">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C45" s="18">
         <v>167</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" s="18">
-        <v>1</v>
+      <c r="D45" s="18">
+        <v>54</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F45" s="18">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C46" s="18">
         <v>175</v>
       </c>
-      <c r="D46" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="18">
-        <v>1</v>
+      <c r="D46" s="18">
+        <v>48</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="F46" s="18">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C47" s="18">
         <v>176</v>
       </c>
-      <c r="D47" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="18">
-        <v>1</v>
+      <c r="D47" s="18">
+        <v>48</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F47" s="18">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C48" s="18">
         <v>215</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48" s="18">
-        <v>1</v>
+      <c r="D48" s="18">
+        <v>80</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F48" s="18">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C49" s="18">
         <v>239</v>
       </c>
-      <c r="D49" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E49" s="18">
+      <c r="D49" s="18">
+        <v>124</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="18">
         <v>2</v>
-      </c>
-      <c r="F49" s="18">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>